<commit_message>
Pequenas melhorias e atualizacao do nome de filipe teotonio. load das provas do google drive tambem.
</commit_message>
<xml_diff>
--- a/leda-submission-server/conf/frequencia_2016.1_1411179-01_074205337.xlsx
+++ b/leda-submission-server/conf/frequencia_2016.1_1411179-01_074205337.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UFCG\leda\leda-tools\leda-submission-server\conf\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Frequencia" r:id="rId3" sheetId="1"/>
+    <sheet name="Frequencia" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -83,9 +90,6 @@
     <t>115111578</t>
   </si>
   <si>
-    <t>FILIPE TEOTÔNIO RAMALHO MENDONÇA</t>
-  </si>
-  <si>
     <t>115111410</t>
   </si>
   <si>
@@ -270,16 +274,18 @@
   </si>
   <si>
     <t>YTALO LUIZ OURIQUES RODRIGUES</t>
+  </si>
+  <si>
+    <t>FILIPE TEOTONIO RAMALHO MENDONCA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -291,7 +297,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -308,31 +314,306 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true">
-      <pane xSplit="3.0" ySplit="2.0" state="frozen" topLeftCell="D3" activePane="bottomRight"/>
-      <selection pane="bottomRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.96484375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.08984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="46.609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -340,9 +621,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -351,9 +632,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2.0</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -362,9 +643,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3.0</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -373,9 +654,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4.0</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -384,9 +665,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5.0</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -395,9 +676,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6.0</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
@@ -406,9 +687,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>7.0</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -417,9 +698,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>8.0</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -428,9 +709,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>9.0</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -439,9 +720,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10.0</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
@@ -450,359 +731,359 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>11.0</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" t="s">
         <v>36</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" t="s">
         <v>50</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" t="s">
         <v>52</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" t="s">
         <v>54</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" t="s">
         <v>56</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" t="s">
         <v>58</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" t="s">
         <v>60</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" t="s">
         <v>62</v>
       </c>
-      <c r="C33" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" t="s">
         <v>64</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" t="s">
         <v>66</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" t="s">
         <v>68</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" t="s">
         <v>70</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" t="s">
         <v>72</v>
       </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" t="s">
         <v>74</v>
       </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>38.0</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" t="s">
         <v>76</v>
       </c>
-      <c r="C40" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" t="s">
         <v>78</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" t="s">
         <v>80</v>
       </c>
-      <c r="C42" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" t="s">
         <v>82</v>
       </c>
-      <c r="C43" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" t="s">
         <v>84</v>
       </c>
-      <c r="C44" t="s">
-        <v>85</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>